<commit_message>
update table to meet with new feature model
</commit_message>
<xml_diff>
--- a/device_family.xlsx
+++ b/device_family.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni_Stuff\Eclipse\workspace\IoTAssistant\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Git\DS_2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t>EN</t>
   </si>
@@ -38,12 +38,6 @@
     <t>SMS</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>Default</t>
-  </si>
-  <si>
     <t>Input</t>
   </si>
   <si>
@@ -65,9 +59,6 @@
     <t>Mouse, Keyboard</t>
   </si>
   <si>
-    <t>Screen</t>
-  </si>
-  <si>
     <t>Visual</t>
   </si>
   <si>
@@ -77,51 +68,50 @@
     <t>Screen, Speakers</t>
   </si>
   <si>
-    <t>Pulse</t>
-  </si>
-  <si>
     <t>Smart Watch</t>
   </si>
   <si>
-    <t>Lamps</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Button</t>
-  </si>
-  <si>
     <t>Auditory</t>
   </si>
   <si>
-    <t>Panic Button</t>
-  </si>
-  <si>
     <t>Movement Sensor</t>
   </si>
   <si>
-    <t>Movement</t>
+    <t>Panic Vest</t>
+  </si>
+  <si>
+    <t>Screen, Light</t>
+  </si>
+  <si>
+    <t>Portable Alarm</t>
+  </si>
+  <si>
+    <t>Patterns</t>
+  </si>
+  <si>
+    <t>Management</t>
+  </si>
+  <si>
+    <t>Management, Emergency Contact</t>
+  </si>
+  <si>
+    <t>Reminders</t>
+  </si>
+  <si>
+    <t>Reminders, Movement Detection</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Webdings"/>
-      <family val="1"/>
-      <charset val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -144,12 +134,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -437,166 +424,169 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>4</v>
+        <v>21</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>12</v>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>4</v>
+        <v>22</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>12</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>4</v>
+        <v>21</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>